<commit_message>
close #37: Check if the indicator is not level zero or negative
</commit_message>
<xml_diff>
--- a/input_data/data_errors/4_descricao/descricao.xlsx
+++ b/input_data/data_errors/4_descricao/descricao.xlsx
@@ -188,7 +188,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -707,7 +707,7 @@
         <v>5000</v>
       </c>
       <c r="B3" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>17</v>
@@ -749,7 +749,7 @@
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="58.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="73.5">
       <c r="A4" s="5">
         <v>5001</v>
       </c>
@@ -796,12 +796,12 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="79.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="100.5">
       <c r="A5" s="5">
         <v>5002</v>
       </c>
       <c r="B5" s="5">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>24</v>
@@ -843,7 +843,7 @@
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="58.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="73.5">
       <c r="A6" s="5">
         <v>5003</v>
       </c>
@@ -890,7 +890,7 @@
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="58.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="73.5">
       <c r="A7" s="5">
         <v>5004</v>
       </c>
@@ -937,7 +937,7 @@
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="79.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="100.5">
       <c r="A8" s="5">
         <v>5005</v>
       </c>
@@ -984,7 +984,7 @@
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="48">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="60">
       <c r="A9" s="5">
         <v>5006</v>
       </c>

</xml_diff>

<commit_message>
close #32: Add check for punctuation in indicator descriptions
</commit_message>
<xml_diff>
--- a/input_data/data_errors/4_descricao/descricao.xlsx
+++ b/input_data/data_errors/4_descricao/descricao.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>codigo</t>
   </si>
@@ -49,7 +49,7 @@
     <t>meta</t>
   </si>
   <si>
-    <t>Segurança Alimentar</t>
+    <t>Segurança Alimentar.</t>
   </si>
   <si>
     <t>Impactos para Segurança Alimentar</t>
@@ -58,7 +58,7 @@
     <t>&lt;h1&gt;Consequências esperadas e resultantes das mudanças climáticas em sistemas  &lt;/h1&gt; socioecológicos relacionados à segurança alimentar</t>
   </si>
   <si>
-    <t>São os efeitos sobre vidas, meioz de subsistência, saúde, ecossistemas, economias, çociedades, culturas, serviços e infraestrutura, devido a alterações climáticas ou eventos climáticos que se dão dentro de períodos específicos de tempo, de vulnerabilidade e de exposição da sociedade ou sistema, relacionados à segurança alimentar.&lt;br&gt;A Segurança Alimentar e Nutricional (SAN) consiste na realização do direito de todos ao acesso regular e permanente a alimentos de qualidade, em quantidade suficiente, sem comprometer o acesso a outras necessidades essenciais, tendo como base práticas alimentares promotoras de saúde, que respeitem a diversidade cultural e que sejam ambiental, cultural, econômica e socialmente sustentáveis.&lt;br&gt;&lt;br&gt;Fontes:&lt;br&gt;&lt;a href="http://www.planalto.gov.br/ccivil_03/_ato2004-2006/2006/lei/l11346.htm"&gt;BRASIL. LEI Nº 11.346, DE 15 DE SETEMBRO DE 2006. Brasília: 2006.&lt;/a&gt;&lt;br&gt;INTERGOVERNMENTAL PANEL ON CLIMATE CHANGE - IPCC. Climate Change 2014: Synthesis Report. Working Groups I, II and III to the Fifth Assessment Report of the Intergovernmental Panel on Climate Change [Core Writing Team, R.K. Pachauri and L.A. Meyer (eds.)]. IPCC, Geneva, Switzerland, 151 pp.</t>
+    <t>São os efeitos sobre vidas, meioz de subsistência, saúde, ecossistemas, economias, çociedades, culturas, serviços e infraestrutura, devido a alterações climáticas ou eventos climáticos que se dão dentro de períodos específicos de tempo, de vulnerabilidade e de exposição da sociedade ou sistema, relacionados à segurança alimentar.&lt;br&gt;A Segurança Alimentar e Nutricional (SAN) consiste na realização do direito de todos ao acesso regular e permanente a alimentos de qualidade, em quantidade suficiente, sem comprometer o acesso a outras necessidades essenciais, tendo como base práticas alimentares promotoras de saúde, que respeitem a diversidade cultural e que sejam ambiental, cultural, econômica e socialmente sustentáveis.&lt;br&gt;&lt;br&gt;Fontes:&lt;br&gt;&lt;a href="http://www.planalto.gov.br/ccivil_03/_ato2004-2006/2006/lei/l11346.htm"&gt;BRASIL. LEI Nº 11.346, DE 15 DE SETEMBRO DE 2006. Brasília: 2006.&lt;/a&gt;&lt;br&gt;INTERGOVERNMENTAL PANEL ON CLIMATE CHANGE - IPCC. Climate Change 2014: Synthesis Report. Working Groups I, II and III to the Fifth Assessment Report of the Intergovernmental Panel on Climate Change [Core Writing Team, R.K. Pachauri and L.A. Meyer (eds.)]. IPCC, Geneva, Switzerland, 151 pp</t>
   </si>
   <si>
     <t>AdaptaBrasil MCTI/INPE</t>
@@ -67,10 +67,10 @@
     <t>6.2,6.3,6.4</t>
   </si>
   <si>
-    <t>Seca</t>
+    <t>Seca.</t>
   </si>
   <si>
-    <t>Índice de Risco de Impacto para Seca</t>
+    <t>Índice de Risco de Impacto para Seca.</t>
   </si>
   <si>
     <t>&lt;strong&gt;Risco de impacto das mudanças climáticas em sistemas&lt;/strong&gt; socioecológicos, considerando a ameaça climática de seca</t>
@@ -82,6 +82,9 @@
     <t>6.2</t>
   </si>
   <si>
+    <t>Seca</t>
+  </si>
+  <si>
     <t>Grau de suscetibilidade de um sistema socioecológico aos efeitos das mudanças climáticas, &lt;br&gt; especificamente aquelas que resultam em seca</t>
   </si>
   <si>
@@ -91,7 +94,7 @@
     <t>Exposição</t>
   </si>
   <si>
-    <t>Índice de Exposição</t>
+    <t>Índice de Exposição.</t>
   </si>
   <si>
     <t>Magnitude do contato entre o sistema socioecológico e as ameaças climáticas relacionadas à seca por meio da distribuição de elementos de superfície</t>
@@ -655,7 +658,7 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="69">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="87">
       <c r="A2" s="4">
         <v>2</v>
       </c>
@@ -702,7 +705,7 @@
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="48">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="60">
       <c r="A3" s="5">
         <v>5000</v>
       </c>
@@ -757,17 +760,17 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="5">
         <v>0</v>
@@ -804,17 +807,17 @@
         <v>-1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H5" s="5">
         <v>0</v>
@@ -826,7 +829,7 @@
         <v>15</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -851,17 +854,17 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" s="5">
         <v>1</v>
@@ -873,7 +876,7 @@
         <v>15</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -898,17 +901,17 @@
         <v>4</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H7" s="5">
         <v>0</v>
@@ -920,7 +923,7 @@
         <v>15</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -945,17 +948,17 @@
         <v>4</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8" s="5">
         <v>0</v>
@@ -967,7 +970,7 @@
         <v>15</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -992,17 +995,17 @@
         <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H9" s="5">
         <v>0</v>
@@ -1014,7 +1017,7 @@
         <v>15</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -1039,17 +1042,17 @@
         <v>5</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H10" s="5">
         <v>0</v>
@@ -1061,7 +1064,7 @@
         <v>15</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>

</xml_diff>

<commit_message>
Update dependencies and fix data cleaning function
</commit_message>
<xml_diff>
--- a/input_data/data_errors/4_descricao/descricao.xlsx
+++ b/input_data/data_errors/4_descricao/descricao.xlsx
@@ -194,7 +194,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -661,7 +661,7 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="69">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="87">
       <c r="A2" s="4">
         <v>2</v>
       </c>
@@ -708,7 +708,7 @@
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="60">
       <c r="A3" s="6">
         <v>5000</v>
       </c>
@@ -755,7 +755,7 @@
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="73.5">
       <c r="A4" s="6">
         <v>5001</v>
       </c>
@@ -802,7 +802,7 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="100.5">
       <c r="A5" s="6">
         <v>5002</v>
       </c>
@@ -849,7 +849,7 @@
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="73.5">
       <c r="A6" s="6">
         <v>5003</v>
       </c>
@@ -896,7 +896,7 @@
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="73.5">
       <c r="A7" s="6">
         <v>5004</v>
       </c>
@@ -943,7 +943,7 @@
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="100.5">
       <c r="A8" s="6">
         <v>5005</v>
       </c>
@@ -990,7 +990,7 @@
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="60">
       <c r="A9" s="6">
         <v>5006</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="60">
       <c r="A10" s="6">
         <v>5007</v>
       </c>
@@ -1084,7 +1084,7 @@
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="60">
       <c r="A11" s="6">
         <v>5007</v>
       </c>
@@ -1131,7 +1131,7 @@
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5"/>
@@ -1158,7 +1158,7 @@
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="5"/>
@@ -1185,7 +1185,7 @@
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
@@ -1212,7 +1212,7 @@
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
@@ -1239,7 +1239,7 @@
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
@@ -1266,7 +1266,7 @@
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
@@ -1293,7 +1293,7 @@
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5"/>
@@ -1320,7 +1320,7 @@
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="5"/>
@@ -1347,7 +1347,7 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="5"/>

</xml_diff>

<commit_message>
Fix file path and add error handling in verify_structure_folder_files function
</commit_message>
<xml_diff>
--- a/input_data/data_errors/4_descricao/descricao.xlsx
+++ b/input_data/data_errors/4_descricao/descricao.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>codigo</t>
   </si>
@@ -170,6 +170,18 @@
   </si>
   <si>
     <t>Características dos produtores ruarais agropecuários</t>
+  </si>
+  <si>
+    <t>MYSQL</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>Produtores rurais casa</t>
+  </si>
+  <si>
+    <t>Características dos produtores ruarais casa agropecuários</t>
   </si>
 </sst>
 </file>
@@ -1132,17 +1144,37 @@
       <c r="Y11" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>

</xml_diff>

<commit_message>
close #79:  Add verify cleanliness of data files in a specified folder
</commit_message>
<xml_diff>
--- a/input_data/data_errors/4_descricao/descricao.xlsx
+++ b/input_data/data_errors/4_descricao/descricao.xlsx
@@ -604,7 +604,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="8" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="6.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="20.862142857142857" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="9" width="49.71928571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="9" width="59.14785714285715" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="9" width="27.862142857142857" customWidth="1" bestFit="1"/>
@@ -731,7 +731,7 @@
         <v>5000</v>
       </c>
       <c r="B3" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>17</v>
@@ -778,7 +778,7 @@
         <v>5001</v>
       </c>
       <c r="B4" s="6">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>17</v>

</xml_diff>